<commit_message>
update final report 2 -- almost done!
</commit_message>
<xml_diff>
--- a/survey/excel/sd4.xlsx
+++ b/survey/excel/sd4.xlsx
@@ -13,12 +13,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'sd4'!$F$1:$H$101</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="110">
   <si>
     <t>Domain</t>
   </si>
@@ -345,6 +344,9 @@
   </si>
   <si>
     <t>Reduction Factor</t>
+  </si>
+  <si>
+    <t>Total Resources</t>
   </si>
 </sst>
 </file>
@@ -958,7 +960,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1959,12 +1961,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:overlap val="100"/>
-        <c:axId val="109617920"/>
-        <c:axId val="109619456"/>
+        <c:axId val="56054912"/>
+        <c:axId val="85411712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109617920"/>
+        <c:axId val="56054912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1973,7 +1974,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109619456"/>
+        <c:crossAx val="85411712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1981,7 +1982,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109619456"/>
+        <c:axId val="85411712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1997,7 +1998,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="109617920"/>
+        <c:crossAx val="56054912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2170,11 +2171,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="113388160"/>
-        <c:axId val="113394432"/>
+        <c:axId val="85442944"/>
+        <c:axId val="114699264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113388160"/>
+        <c:axId val="85442944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2203,7 +2204,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113394432"/>
+        <c:crossAx val="114699264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2211,7 +2212,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113394432"/>
+        <c:axId val="114699264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2241,7 +2242,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113388160"/>
+        <c:crossAx val="85442944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2288,6 +2289,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2389,11 +2391,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="113419392"/>
-        <c:axId val="113421312"/>
+        <c:axId val="115316992"/>
+        <c:axId val="115357184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113419392"/>
+        <c:axId val="115316992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2415,12 +2417,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113421312"/>
+        <c:crossAx val="115357184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2428,7 +2431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113421312"/>
+        <c:axId val="115357184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2451,13 +2454,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113419392"/>
+        <c:crossAx val="115316992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2886,11 +2890,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="113546752"/>
-        <c:axId val="113548672"/>
+        <c:axId val="146873728"/>
+        <c:axId val="148256256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113546752"/>
+        <c:axId val="146873728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2923,12 +2927,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113548672"/>
+        <c:crossAx val="148256256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113548672"/>
+        <c:axId val="148256256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2958,7 +2962,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113546752"/>
+        <c:crossAx val="146873728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3390,11 +3394,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="113565056"/>
-        <c:axId val="116598272"/>
+        <c:axId val="148719872"/>
+        <c:axId val="160117120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113565056"/>
+        <c:axId val="148719872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3428,12 +3432,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116598272"/>
+        <c:crossAx val="160117120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116598272"/>
+        <c:axId val="160117120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3463,11 +3467,1736 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113565056"/>
+        <c:crossAx val="148719872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Synonym Url Sets and Reduced URLs compared to Total Resources by Site</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'sd4'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Syn URL Sets</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'sd4'!$A$2:$A$85</c:f>
+              <c:strCache>
+                <c:ptCount val="84"/>
+                <c:pt idx="0">
+                  <c:v>rakuten.co.jp</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dailymotion.com</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>163.com</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>sina.com.cn</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>sohu.com</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>youku.com</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>huffingtonpost.com</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>amazon.co.uk</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>qq.com</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>people.com.cn</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>taobao.com</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>cnn.com</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>ebay.de</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>ebay.com</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>ebay.co.uk</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>amazon.cn</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>chinadaily.com.cn</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>gmw.cn</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>imdb.com</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>microsoft.com</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>wikia.com</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>aliexpress.com</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>imgur.com</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>naver.com</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>xhamster.com</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>hao123.com</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>nicovideo.jp</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>tudou.com</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>fc2.com</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>adcash.com</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>pornhub.com</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>youtube.com</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>amazon.co.jp</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>ask.com</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>amazon.de</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>bbc.co.uk</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>go.com</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>xvideos.com</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>amazon.com</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>diply.com</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>espn.go.com</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>adobe.com</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>alipay.com</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>reddit.com</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>360.cn</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>flipkart.com</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>tmall.com</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>apple.com</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>yahoo.co.jp</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>yandex.ru</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>stackoverflow.com</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>msn.com</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>vk.com</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>alibaba.com</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>cntv.cn</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>wikipedia.org</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>netflix.com</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>soso.com</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>blogger.com</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>blogspot.com</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>craigslist.org</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>google.com.br</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>google.com.tr</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>google.it</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>google.pl</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>googleadservices.com</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>google.ca</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>google.co.in</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>google.co.jp</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>google.com</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>google.com.au</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>google.com.mx</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>google.co.uk</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>google.de</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>google.es</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>google.fr</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>google.ru</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>google.com.hk</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>onclickads.net</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>weibo.com</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>bing.com</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>t.co</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>baidu.com</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>youradexchange.com</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'sd4'!$B$2:$B$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="84"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'sd4'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Reduced URLs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'sd4'!$A$2:$A$85</c:f>
+              <c:strCache>
+                <c:ptCount val="84"/>
+                <c:pt idx="0">
+                  <c:v>rakuten.co.jp</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dailymotion.com</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>163.com</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>sina.com.cn</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>sohu.com</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>youku.com</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>huffingtonpost.com</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>amazon.co.uk</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>qq.com</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>people.com.cn</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>taobao.com</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>cnn.com</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>ebay.de</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>ebay.com</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>ebay.co.uk</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>amazon.cn</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>chinadaily.com.cn</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>gmw.cn</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>imdb.com</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>microsoft.com</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>wikia.com</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>aliexpress.com</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>imgur.com</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>naver.com</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>xhamster.com</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>hao123.com</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>nicovideo.jp</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>tudou.com</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>fc2.com</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>adcash.com</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>pornhub.com</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>youtube.com</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>amazon.co.jp</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>ask.com</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>amazon.de</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>bbc.co.uk</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>go.com</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>xvideos.com</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>amazon.com</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>diply.com</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>espn.go.com</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>adobe.com</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>alipay.com</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>reddit.com</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>360.cn</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>flipkart.com</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>tmall.com</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>apple.com</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>yahoo.co.jp</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>yandex.ru</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>stackoverflow.com</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>msn.com</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>vk.com</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>alibaba.com</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>cntv.cn</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>wikipedia.org</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>netflix.com</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>soso.com</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>blogger.com</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>blogspot.com</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>craigslist.org</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>google.com.br</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>google.com.tr</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>google.it</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>google.pl</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>googleadservices.com</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>google.ca</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>google.co.in</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>google.co.jp</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>google.com</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>google.com.au</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>google.com.mx</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>google.co.uk</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>google.de</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>google.es</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>google.fr</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>google.ru</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>google.com.hk</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>onclickads.net</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>weibo.com</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>bing.com</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>t.co</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>baidu.com</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>youradexchange.com</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'sd4'!$C$2:$C$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="84"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'sd4'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Resources</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'sd4'!$A$2:$A$85</c:f>
+              <c:strCache>
+                <c:ptCount val="84"/>
+                <c:pt idx="0">
+                  <c:v>rakuten.co.jp</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dailymotion.com</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>163.com</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>sina.com.cn</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>sohu.com</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>youku.com</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>huffingtonpost.com</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>amazon.co.uk</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>qq.com</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>people.com.cn</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>taobao.com</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>cnn.com</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>ebay.de</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>ebay.com</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>ebay.co.uk</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>amazon.cn</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>chinadaily.com.cn</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>gmw.cn</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>imdb.com</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>microsoft.com</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>wikia.com</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>aliexpress.com</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>imgur.com</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>naver.com</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>xhamster.com</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>hao123.com</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>nicovideo.jp</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>tudou.com</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>fc2.com</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>adcash.com</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>pornhub.com</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>youtube.com</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>amazon.co.jp</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>ask.com</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>amazon.de</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>bbc.co.uk</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>go.com</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>xvideos.com</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>amazon.com</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>diply.com</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>espn.go.com</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>adobe.com</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>alipay.com</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>reddit.com</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>360.cn</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>flipkart.com</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>tmall.com</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>apple.com</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>yahoo.co.jp</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>yandex.ru</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>stackoverflow.com</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>msn.com</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>vk.com</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>alibaba.com</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>cntv.cn</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>wikipedia.org</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>netflix.com</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>soso.com</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>blogger.com</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>blogspot.com</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>craigslist.org</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>google.com.br</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>google.com.tr</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>google.it</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>google.pl</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>googleadservices.com</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>google.ca</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>google.co.in</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>google.co.jp</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>google.com</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>google.com.au</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>google.com.mx</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>google.co.uk</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>google.de</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>google.es</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>google.fr</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>google.ru</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>google.com.hk</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>onclickads.net</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>weibo.com</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>bing.com</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>t.co</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>baidu.com</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>youradexchange.com</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'sd4'!$D$2:$D$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="84"/>
+                <c:pt idx="0">
+                  <c:v>754</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>413.77777777777698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>385.888888888888</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>305.375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>304.83333333333297</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>271.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>261.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>220.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>202.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>197.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>169.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>168.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>163.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>158.666666666666</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>155.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>120.555555555555</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>114.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>107.2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>89.6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>89.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>87.625</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>75.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>64.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>60.8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>56.6</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>55.9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>54.9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>54.1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>53.7</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>52.3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>41.7</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>38.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>34.1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>24.1</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>19.2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:overlap val="-25"/>
+        <c:axId val="44257280"/>
+        <c:axId val="44259584"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="44257280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="44259584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="44259584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9525">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="44257280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3627,6 +5356,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>714374</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3924,8 +5683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I55"/>
+    <sheetView tabSelected="1" topLeftCell="H50" workbookViewId="0">
+      <selection activeCell="D85" sqref="A1:D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3947,6 +5706,9 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>109</v>
+      </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
@@ -3977,13 +5739,16 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C2">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="D2">
+        <v>754</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -4016,13 +5781,16 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>107</v>
+      </c>
+      <c r="D3">
+        <v>413.77777777777698</v>
       </c>
       <c r="F3" t="s">
         <v>83</v>
@@ -4055,13 +5823,16 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>385.888888888888</v>
       </c>
       <c r="F4" t="s">
         <v>26</v>
@@ -4094,13 +5865,16 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>305.375</v>
       </c>
       <c r="F5" t="s">
         <v>57</v>
@@ -4133,13 +5907,16 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>304.83333333333297</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -4172,13 +5949,16 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="B7">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>63</v>
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>271.7</v>
       </c>
       <c r="F7" t="s">
         <v>23</v>
@@ -4211,13 +5991,16 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>261.60000000000002</v>
       </c>
       <c r="F8" t="s">
         <v>77</v>
@@ -4250,13 +6033,16 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9">
         <v>2</v>
+      </c>
+      <c r="D9">
+        <v>220.1</v>
       </c>
       <c r="F9" t="s">
         <v>100</v>
@@ -4282,13 +6068,16 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>219</v>
       </c>
       <c r="F10" t="s">
         <v>3</v>
@@ -4311,13 +6100,16 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="B11">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>27</v>
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>202.3</v>
       </c>
       <c r="F11" t="s">
         <v>36</v>
@@ -4340,13 +6132,16 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>46</v>
+      </c>
+      <c r="D12">
+        <v>197.3</v>
       </c>
       <c r="F12" t="s">
         <v>79</v>
@@ -4367,13 +6162,16 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>34</v>
+      </c>
+      <c r="D13">
+        <v>169.6</v>
       </c>
       <c r="F13" t="s">
         <v>80</v>
@@ -4394,13 +6192,16 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>168.75</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
@@ -4421,13 +6222,16 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B15">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>163.80000000000001</v>
       </c>
       <c r="F15" t="s">
         <v>65</v>
@@ -4448,13 +6252,16 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>158.666666666666</v>
       </c>
       <c r="F16" t="s">
         <v>22</v>
@@ -4475,13 +6282,16 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>155.4</v>
       </c>
       <c r="F17" t="s">
         <v>34</v>
@@ -4502,13 +6312,16 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>137</v>
       </c>
       <c r="F18" t="s">
         <v>75</v>
@@ -4526,13 +6339,16 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>120.555555555555</v>
       </c>
       <c r="F19" t="s">
         <v>91</v>
@@ -4550,13 +6366,16 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="D20">
+        <v>114.9</v>
       </c>
       <c r="F20" t="s">
         <v>56</v>
@@ -4574,13 +6393,16 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21">
         <v>9</v>
+      </c>
+      <c r="D21">
+        <v>107.2</v>
       </c>
       <c r="F21" t="s">
         <v>59</v>
@@ -4598,13 +6420,16 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="B22">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>34</v>
+        <v>9</v>
+      </c>
+      <c r="D22">
+        <v>100</v>
       </c>
       <c r="F22" t="s">
         <v>69</v>
@@ -4622,13 +6447,16 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="D23">
+        <v>96</v>
       </c>
       <c r="F23" t="s">
         <v>29</v>
@@ -4646,13 +6474,16 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>89.6</v>
       </c>
       <c r="F24" t="s">
         <v>58</v>
@@ -4670,13 +6501,16 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="B25">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C25">
-        <v>107</v>
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>89.5</v>
       </c>
       <c r="F25" t="s">
         <v>73</v>
@@ -4694,13 +6528,16 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>89</v>
       </c>
       <c r="F26" t="s">
         <v>85</v>
@@ -4718,13 +6555,16 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="D27">
+        <v>87.625</v>
       </c>
       <c r="F27" t="s">
         <v>31</v>
@@ -4742,13 +6582,16 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C28">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="D28">
+        <v>77</v>
       </c>
       <c r="F28" t="s">
         <v>37</v>
@@ -4766,13 +6609,16 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>75.099999999999994</v>
       </c>
       <c r="F29" t="s">
         <v>67</v>
@@ -4790,13 +6636,16 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C30">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="D30">
+        <v>64.2</v>
       </c>
       <c r="F30" t="s">
         <v>4</v>
@@ -4814,13 +6663,16 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>64</v>
       </c>
       <c r="F31" t="s">
         <v>5</v>
@@ -4838,13 +6690,16 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="D32">
+        <v>63</v>
       </c>
       <c r="F32" t="s">
         <v>11</v>
@@ -4862,13 +6717,16 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="B33">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C33">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>60.8</v>
       </c>
       <c r="F33" t="s">
         <v>30</v>
@@ -4886,13 +6744,16 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34">
         <v>3</v>
+      </c>
+      <c r="D34">
+        <v>57.1</v>
       </c>
       <c r="F34" t="s">
         <v>66</v>
@@ -4910,13 +6771,16 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35">
         <v>16</v>
       </c>
-      <c r="C35">
-        <v>18</v>
+      <c r="D35">
+        <v>56.6</v>
       </c>
       <c r="F35" t="s">
         <v>89</v>
@@ -4934,13 +6798,16 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>56</v>
       </c>
       <c r="F36" t="s">
         <v>97</v>
@@ -4958,13 +6825,16 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>55.9</v>
       </c>
       <c r="F37" t="s">
         <v>99</v>
@@ -4982,13 +6852,16 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>54.9</v>
       </c>
       <c r="F38" t="s">
         <v>6</v>
@@ -5006,13 +6879,16 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="C39">
         <v>0</v>
+      </c>
+      <c r="D39">
+        <v>54.1</v>
       </c>
       <c r="F39" t="s">
         <v>7</v>
@@ -5030,13 +6906,16 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="D40">
+        <v>53.7</v>
       </c>
       <c r="F40" t="s">
         <v>10</v>
@@ -5054,13 +6933,16 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41">
         <v>0</v>
+      </c>
+      <c r="D41">
+        <v>52.3</v>
       </c>
       <c r="F41" t="s">
         <v>13</v>
@@ -5078,13 +6960,16 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>51</v>
       </c>
       <c r="F42" t="s">
         <v>14</v>
@@ -5102,13 +6987,16 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>46</v>
       </c>
       <c r="F43" t="s">
         <v>35</v>
@@ -5126,13 +7014,16 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>44</v>
       </c>
       <c r="F44" t="s">
         <v>71</v>
@@ -5150,13 +7041,16 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>41.7</v>
       </c>
       <c r="F45" t="s">
         <v>78</v>
@@ -5174,13 +7068,16 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>41</v>
       </c>
       <c r="F46" t="s">
         <v>82</v>
@@ -5198,13 +7095,16 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>38.200000000000003</v>
       </c>
       <c r="F47" t="s">
         <v>86</v>
@@ -5222,13 +7122,16 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D48">
+        <v>34.1</v>
       </c>
       <c r="F48" t="s">
         <v>9</v>
@@ -5246,13 +7149,16 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>32</v>
       </c>
       <c r="F49" t="s">
         <v>15</v>
@@ -5270,13 +7176,16 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>32</v>
       </c>
       <c r="F50" t="s">
         <v>18</v>
@@ -5294,13 +7203,16 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <v>32</v>
       </c>
       <c r="F51" t="s">
         <v>32</v>
@@ -5318,13 +7230,16 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>27.5</v>
       </c>
       <c r="F52" t="s">
         <v>76</v>
@@ -5342,13 +7257,16 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D53">
+        <v>27</v>
       </c>
       <c r="F53" t="s">
         <v>90</v>
@@ -5366,13 +7284,16 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D54">
+        <v>25</v>
       </c>
       <c r="F54" t="s">
         <v>94</v>
@@ -5390,13 +7311,16 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="B55">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C55">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>24.1</v>
       </c>
       <c r="F55" t="s">
         <v>102</v>
@@ -5414,13 +7338,16 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B56">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C56">
-        <v>50</v>
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>20</v>
       </c>
       <c r="F56" t="s">
         <v>17</v>
@@ -5434,13 +7361,16 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="B57">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C57">
-        <v>22</v>
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>20</v>
       </c>
       <c r="F57" t="s">
         <v>19</v>
@@ -5454,13 +7384,16 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B58">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C58">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>19.2</v>
       </c>
       <c r="F58" t="s">
         <v>20</v>
@@ -5474,13 +7407,16 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="B59">
         <v>0</v>
       </c>
       <c r="C59">
         <v>0</v>
+      </c>
+      <c r="D59">
+        <v>19</v>
       </c>
       <c r="F59" t="s">
         <v>21</v>
@@ -5494,13 +7430,16 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="B60">
         <v>0</v>
       </c>
       <c r="C60">
         <v>0</v>
+      </c>
+      <c r="D60">
+        <v>10</v>
       </c>
       <c r="F60" t="s">
         <v>24</v>
@@ -5514,13 +7453,16 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="B61">
         <v>0</v>
       </c>
       <c r="C61">
         <v>0</v>
+      </c>
+      <c r="D61">
+        <v>10</v>
       </c>
       <c r="F61" t="s">
         <v>25</v>
@@ -5534,13 +7476,16 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="B62">
         <v>0</v>
       </c>
       <c r="C62">
         <v>0</v>
+      </c>
+      <c r="D62">
+        <v>10</v>
       </c>
       <c r="F62" t="s">
         <v>27</v>
@@ -5554,13 +7499,16 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B63">
         <v>0</v>
       </c>
       <c r="C63">
         <v>0</v>
+      </c>
+      <c r="D63">
+        <v>9</v>
       </c>
       <c r="F63" t="s">
         <v>28</v>
@@ -5574,12 +7522,15 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B64">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
         <v>9</v>
       </c>
       <c r="F64" t="s">
@@ -5594,13 +7545,16 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>9</v>
       </c>
       <c r="F65" t="s">
         <v>38</v>
@@ -5614,13 +7568,16 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B66">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C66">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>9</v>
       </c>
       <c r="F66" t="s">
         <v>39</v>
@@ -5634,13 +7591,16 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="C67">
         <v>0</v>
+      </c>
+      <c r="D67">
+        <v>8</v>
       </c>
       <c r="F67" t="s">
         <v>40</v>
@@ -5654,13 +7614,16 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="B68">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C68">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>8</v>
       </c>
       <c r="F68" t="s">
         <v>41</v>
@@ -5674,13 +7637,16 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="C69">
         <v>0</v>
+      </c>
+      <c r="D69">
+        <v>8</v>
       </c>
       <c r="F69" t="s">
         <v>42</v>
@@ -5694,13 +7660,16 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="B70">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C70">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>8</v>
       </c>
       <c r="F70" t="s">
         <v>43</v>
@@ -5714,13 +7683,16 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="B71">
         <v>0</v>
       </c>
       <c r="C71">
         <v>0</v>
+      </c>
+      <c r="D71">
+        <v>8</v>
       </c>
       <c r="F71" t="s">
         <v>44</v>
@@ -5734,13 +7706,16 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="B72">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C72">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>8</v>
       </c>
       <c r="F72" t="s">
         <v>45</v>
@@ -5754,13 +7729,16 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="B73">
         <v>0</v>
       </c>
       <c r="C73">
         <v>0</v>
+      </c>
+      <c r="D73">
+        <v>8</v>
       </c>
       <c r="F73" t="s">
         <v>46</v>
@@ -5774,13 +7752,16 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
         <v>8</v>
-      </c>
-      <c r="C74">
-        <v>11</v>
       </c>
       <c r="F74" t="s">
         <v>47</v>
@@ -5794,13 +7775,16 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C75">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>8</v>
       </c>
       <c r="F75" t="s">
         <v>48</v>
@@ -5814,13 +7798,16 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B76">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C76">
-        <v>32</v>
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>8</v>
       </c>
       <c r="F76" t="s">
         <v>49</v>
@@ -5834,13 +7821,16 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="B77">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C77">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>8</v>
       </c>
       <c r="F77" t="s">
         <v>50</v>
@@ -5854,13 +7844,16 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="B78">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C78">
-        <v>22</v>
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>8</v>
       </c>
       <c r="F78" t="s">
         <v>51</v>
@@ -5874,13 +7867,16 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="B79">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C79">
-        <v>24</v>
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>7</v>
       </c>
       <c r="F79" t="s">
         <v>52</v>
@@ -5894,13 +7890,16 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D80">
+        <v>5.6</v>
       </c>
       <c r="F80" t="s">
         <v>53</v>
@@ -5914,13 +7913,16 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>4</v>
       </c>
       <c r="F81" t="s">
         <v>54</v>
@@ -5934,13 +7936,16 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B82">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C82">
-        <v>46</v>
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
       </c>
       <c r="F82" t="s">
         <v>55</v>
@@ -5962,6 +7967,9 @@
       <c r="C83">
         <v>0</v>
       </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
       <c r="F83" t="s">
         <v>60</v>
       </c>
@@ -5974,13 +7982,16 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="B84">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C84">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
       </c>
       <c r="F84" t="s">
         <v>61</v>
@@ -5994,13 +8005,16 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="B85">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C85">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
       </c>
       <c r="F85" t="s">
         <v>62</v>
@@ -6014,12 +8028,15 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="B86">
         <v>0</v>
       </c>
       <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
         <v>0</v>
       </c>
       <c r="F86" t="s">
@@ -6034,12 +8051,15 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
       <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
         <v>0</v>
       </c>
       <c r="F87" t="s">
@@ -6054,13 +8074,16 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="B88">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C88">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
       </c>
       <c r="F88" t="s">
         <v>68</v>
@@ -6074,13 +8097,16 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
       </c>
       <c r="F89" t="s">
         <v>70</v>
@@ -6094,13 +8120,16 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="B90">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C90">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
       </c>
       <c r="F90" t="s">
         <v>72</v>
@@ -6114,12 +8143,15 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="B91">
         <v>0</v>
       </c>
       <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
         <v>0</v>
       </c>
       <c r="F91" t="s">
@@ -6134,12 +8166,15 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="B92">
         <v>0</v>
       </c>
       <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
         <v>0</v>
       </c>
       <c r="F92" t="s">
@@ -6154,13 +8189,16 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="B93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C93">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
       </c>
       <c r="F93" t="s">
         <v>84</v>
@@ -6174,12 +8212,15 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="B94">
         <v>0</v>
       </c>
       <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
         <v>0</v>
       </c>
       <c r="F94" t="s">
@@ -6194,12 +8235,15 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B95">
         <v>0</v>
       </c>
       <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
         <v>0</v>
       </c>
       <c r="F95" t="s">
@@ -6214,13 +8258,16 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="B96">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C96">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
       </c>
       <c r="F96" t="s">
         <v>92</v>
@@ -6234,12 +8281,15 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B97">
         <v>0</v>
       </c>
       <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
         <v>0</v>
       </c>
       <c r="F97" t="s">
@@ -6254,13 +8304,16 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B98">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C98">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
       </c>
       <c r="F98" t="s">
         <v>95</v>
@@ -6274,13 +8327,16 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B99">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C99">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
       </c>
       <c r="F99" t="s">
         <v>96</v>
@@ -6294,12 +8350,15 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B100">
         <v>0</v>
       </c>
       <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
         <v>0</v>
       </c>
       <c r="F100" t="s">
@@ -6314,13 +8373,16 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
       </c>
       <c r="F101" t="s">
         <v>101</v>
@@ -6334,8 +8396,8 @@
     </row>
   </sheetData>
   <autoFilter ref="F1:H101"/>
-  <sortState ref="N3:N8">
-    <sortCondition ref="N2"/>
+  <sortState ref="A2:D101">
+    <sortCondition descending="1" ref="D2:D101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>